<commit_message>
Login Tests with Select
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/users-for-way2automation-test.xlsx
+++ b/src/test/resources/excel/users-for-way2automation-test.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psi33\eclipse-workspace\NewMavenProject\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3FF75D-DA34-4C83-820A-C488AA876BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175B78E0-1310-4816-A672-7D91B7350ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13530" yWindow="75" windowWidth="15270" windowHeight="14790" activeTab="1" xr2:uid="{5FBF49B0-C76D-4F1A-B8BE-A684CBE6A83E}"/>
+    <workbookView xWindow="13530" yWindow="75" windowWidth="15270" windowHeight="14790" activeTab="2" xr2:uid="{5FBF49B0-C76D-4F1A-B8BE-A684CBE6A83E}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="SecondTest" sheetId="2" r:id="rId2"/>
+    <sheet name="addCustomerTest" sheetId="2" r:id="rId2"/>
+    <sheet name="openAccountTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -79,6 +80,27 @@
   </si>
   <si>
     <t>Hanson</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Fisher</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Joe Smith</t>
+  </si>
+  <si>
+    <t>Dollar</t>
   </si>
 </sst>
 </file>
@@ -496,36 +518,87 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238C12E7-A592-4BE2-B2BC-500714F6AC48}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>56789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>45678</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C87B06-FA7C-4CB2-8A4E-CEDBB21BBCA4}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>